<commit_message>
topic labels, column widths
</commit_message>
<xml_diff>
--- a/topics-k66.xlsx
+++ b/topics-k66.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evanodell/Documents/Code/all-women-shortlists/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD32EA25-A86C-3C4C-9846-B9E876E639A5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F5A3058-2FE4-D443-98D5-98E09ECF2E78}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="340" yWindow="460" windowWidth="28100" windowHeight="16380" xr2:uid="{4429A423-80BE-9046-9A14-897357C39B79}"/>
   </bookViews>
@@ -234,7 +234,7 @@
     <t>Social care</t>
   </si>
   <si>
-    <t>Media and animals</t>
+    <t>Media &amp; animals</t>
   </si>
 </sst>
 </file>
@@ -2413,7 +2413,7 @@
       </c>
       <c r="I69" t="str">
         <f t="shared" si="1"/>
-        <v>"Topic 65" = "(65) Media and animals",</v>
+        <v>"Topic 65" = "(65) Media &amp; animals",</v>
       </c>
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.2">

</xml_diff>